<commit_message>
Add a new extent report
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/_ScenarioResults.xlsx
+++ b/src/test/java/apachePOI/resource/_ScenarioResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="10">
   <si>
     <t>Add -  Edit and Delete Position Category From Excel</t>
   </si>
@@ -1203,7 +1203,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -2809,6 +2809,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="146">
+      <c r="A146" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B146" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B147" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>